<commit_message>
Added additional pivot row for "our" campus. Updated Schedule C formula to subtract values when "our" and "their" campus are same.
</commit_message>
<xml_diff>
--- a/src/main/resources/org/cdlib/ill/report/ScheduleC_Template.xlsx
+++ b/src/main/resources/org/cdlib/ill/report/ScheduleC_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmorrisp/NetBeansProjects/ill-reports/src/main/resources/org/cdlib/ill/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{11263A7E-6ADB-9346-8636-2FF0325DBFAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="27640" windowHeight="15980"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="27640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule C" sheetId="1" r:id="rId1"/>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -508,10 +509,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -579,19 +582,19 @@
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$B$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Lending Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$B$8</f>
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$C$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$C$8</f>
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$8</f>
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$8</f>
         <v>0</v>
       </c>
     </row>
@@ -600,19 +603,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$B$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Lending Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$B$9</f>
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$C$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$C$9</f>
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$9</f>
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$9</f>
         <v>0</v>
       </c>
     </row>
@@ -621,19 +624,19 @@
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$B$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Lending Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$B$10</f>
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$C$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$C$10</f>
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$10</f>
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$10</f>
         <v>0</v>
       </c>
     </row>
@@ -642,19 +645,19 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$B$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Lending Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$B$11</f>
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$C$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$C$11</f>
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$11</f>
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$11</f>
         <v>0</v>
       </c>
     </row>
@@ -663,19 +666,19 @@
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$B$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Lending Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$B$12</f>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$C$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$C$12</f>
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$12</f>
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$12</f>
         <v>0</v>
       </c>
     </row>
@@ -684,19 +687,19 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$B$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Lending Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$B$13</f>
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$C$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$C$13</f>
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$13</f>
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$13</f>
         <v>0</v>
       </c>
     </row>
@@ -705,19 +708,19 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$B$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Lending Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$B$14</f>
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$C$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$C$14</f>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$14</f>
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$14</f>
         <v>0</v>
       </c>
     </row>
@@ -726,19 +729,19 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$B$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Lending Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$B$15</f>
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$C$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$C$15</f>
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$15</f>
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$15</f>
         <v>0</v>
       </c>
     </row>
@@ -747,19 +750,19 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$B$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Lending Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$B$16</f>
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$C$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$C$16</f>
         <v>0</v>
       </c>
       <c r="D16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$16</f>
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$16</f>
         <v>0</v>
       </c>
     </row>
@@ -768,19 +771,19 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$B$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Lending Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$B$17</f>
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$C$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$C$17</f>
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$17</f>
         <v>0</v>
       </c>
       <c r="E17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$17</f>
         <v>0</v>
       </c>
     </row>
@@ -790,12 +793,12 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Loan"),0)+Adjustments!$C$18</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Borrowing Campus", "NRLF", "Loan Service", "Loan"),0)+Adjustments!$C$18</f>
         <v>0</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$18</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Borrowing Campus", "NRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$18</f>
         <v>0</v>
       </c>
     </row>
@@ -805,12 +808,12 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Loan"),0)+Adjustments!$C$19</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Borrowing Campus", "SRLF", "Loan Service", "Loan"),0)+Adjustments!$C$19</f>
         <v>0</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$19</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Borrowing Campus", "SRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$19</f>
         <v>0</v>
       </c>
     </row>
@@ -900,7 +903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1232,7 +1235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1244,7 +1247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1256,7 +1259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1268,7 +1271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1280,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1292,7 +1295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Reverted redundant "our" campus from Schedule C.
</commit_message>
<xml_diff>
--- a/src/main/resources/org/cdlib/ill/report/ScheduleC_Template.xlsx
+++ b/src/main/resources/org/cdlib/ill/report/ScheduleC_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmorrisp/NetBeansProjects/ill-reports/src/main/resources/org/cdlib/ill/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{11263A7E-6ADB-9346-8636-2FF0325DBFAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="27640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="27640" windowHeight="15980"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule C" sheetId="1" r:id="rId1"/>
@@ -115,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -509,12 +508,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -582,19 +579,19 @@
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Lending Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$B$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$B$8</f>
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Borrowing Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$C$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Loan"),0)+Adjustments!$C$8</f>
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$8</f>
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Borrowing Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$8</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$8</f>
         <v>0</v>
       </c>
     </row>
@@ -603,19 +600,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Lending Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$B$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$B$9</f>
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Borrowing Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$C$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Loan"),0)+Adjustments!$C$9</f>
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$9</f>
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Borrowing Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$9</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$9</f>
         <v>0</v>
       </c>
     </row>
@@ -624,19 +621,19 @@
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Lending Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$B$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$B$10</f>
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Borrowing Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$C$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Loan"),0)+Adjustments!$C$10</f>
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$10</f>
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Borrowing Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$10</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCI", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$10</f>
         <v>0</v>
       </c>
     </row>
@@ -645,19 +642,19 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Lending Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$B$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$B$11</f>
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Borrowing Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$C$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Loan"),0)+Adjustments!$C$11</f>
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$11</f>
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Borrowing Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$11</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCLA", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$11</f>
         <v>0</v>
       </c>
     </row>
@@ -666,19 +663,19 @@
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Lending Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$B$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$B$12</f>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Borrowing Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$C$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Loan"),0)+Adjustments!$C$12</f>
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$12</f>
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Borrowing Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$12</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCM", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$12</f>
         <v>0</v>
       </c>
     </row>
@@ -687,19 +684,19 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Lending Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$B$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$B$13</f>
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Borrowing Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$C$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Loan"),0)+Adjustments!$C$13</f>
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$13</f>
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Borrowing Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$13</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCR", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$13</f>
         <v>0</v>
       </c>
     </row>
@@ -708,19 +705,19 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Lending Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$B$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$B$14</f>
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Borrowing Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$C$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Loan"),0)+Adjustments!$C$14</f>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$14</f>
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Borrowing Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$14</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSD", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$14</f>
         <v>0</v>
       </c>
     </row>
@@ -729,19 +726,19 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Lending Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$B$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$B$15</f>
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Borrowing Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$C$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Loan"),0)+Adjustments!$C$15</f>
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$15</f>
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Borrowing Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$15</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$15</f>
         <v>0</v>
       </c>
     </row>
@@ -750,19 +747,19 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Lending Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$B$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$B$16</f>
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Borrowing Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$C$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Loan"),0)+Adjustments!$C$16</f>
         <v>0</v>
       </c>
       <c r="D16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$16</f>
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Borrowing Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$16</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSB", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$16</f>
         <v>0</v>
       </c>
     </row>
@@ -771,19 +768,19 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Lending Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$B$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$B$17</f>
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Borrowing Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$C$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Loan"),0)+Adjustments!$C$17</f>
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'Lending Rollup'!$A$1, "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$D$17</f>
         <v>0</v>
       </c>
       <c r="E17" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Borrowing Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$17</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "UCSC", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$17</f>
         <v>0</v>
       </c>
     </row>
@@ -793,12 +790,12 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Borrowing Campus", "NRLF", "Loan Service", "Loan"),0)+Adjustments!$C$18</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Loan"),0)+Adjustments!$C$18</f>
         <v>0</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Borrowing Campus", "NRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$18</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "NRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$18</f>
         <v>0</v>
       </c>
     </row>
@@ -808,12 +805,12 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Loan"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Borrowing Campus", "SRLF", "Loan Service", "Loan"),0)+Adjustments!$C$19</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Loan"),0)+Adjustments!$C$19</f>
         <v>0</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2">
-        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Copy non returnable"),0)-IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Borrowing Campus", "SRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$19</f>
+        <f>IFERROR(GETPIVOTDATA("Total", 'UC Borrowing Rollup'!$A$1, "Lending Campus", "SRLF", "Loan Service", "Copy non returnable"),0)+Adjustments!$E$19</f>
         <v>0</v>
       </c>
     </row>
@@ -903,7 +900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1235,7 +1232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1247,7 +1244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1259,7 +1256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1271,7 +1268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1283,7 +1280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1295,7 +1292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>